<commit_message>
add hypothetical scenario with vaccination and travel ban to testing scenario
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_new_1.xlsx
+++ b/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_new_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27000" windowHeight="12510" tabRatio="648" firstSheet="1" activeTab="4"/>
+    <workbookView windowHeight="17850" tabRatio="648" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="342">
   <si>
     <t>Template v13.2</t>
   </si>
@@ -1180,11 +1180,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1223,14 +1223,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1238,15 +1230,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1261,14 +1246,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1276,24 +1253,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1301,14 +1263,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1329,8 +1284,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1338,23 +1308,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1367,8 +1321,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1415,7 +1415,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1427,13 +1427,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1445,7 +1463,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1457,19 +1481,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1481,25 +1493,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1517,7 +1517,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1529,13 +1535,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1547,19 +1553,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1577,25 +1577,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1693,57 +1693,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1764,16 +1729,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1786,149 +1777,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2385,8 +2385,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -2672,26 +2672,46 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="4">
+        <v>43915</v>
+      </c>
+      <c r="C14" s="4">
+        <v>44095</v>
+      </c>
+      <c r="D14" s="3">
+        <v>20</v>
+      </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F14" s="3"/>
+        <v>%</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="4">
+        <v>43891</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44089</v>
+      </c>
+      <c r="D15" s="3">
+        <v>80</v>
+      </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F15" s="3"/>
+        <v>%</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3"/>
@@ -5996,8 +6016,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="5"/>
@@ -6064,7 +6084,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="3">
-        <v>0.03</v>
+        <v>0.049</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>67</v>
@@ -6790,7 +6810,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -7216,7 +7236,7 @@
         <v>178</v>
       </c>
       <c r="C28" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>179</v>
@@ -7228,13 +7248,13 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" ht="16.5" spans="1:6">
+    <row r="29" spans="1:6">
       <c r="A29" s="20"/>
       <c r="B29" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C29" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>70</v>

</xml_diff>